<commit_message>
up to 2082/06/08 done
</commit_message>
<xml_diff>
--- a/InvigilatorLlist  Of  Second Terminal Exmination 2082 final.xlsx
+++ b/InvigilatorLlist  Of  Second Terminal Exmination 2082 final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\2nd term exam 2082\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{355477E4-D2D7-41DC-9872-6EA5FEAF38AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821673A0-76BF-4FAA-A6B0-ED7CB698277D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AC1A86C9-541B-43C9-82A5-752D02C01C0B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="65">
   <si>
     <t>GREEN SOCIETY PUBLIC SCHOOL</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>Exam Co-ordinator</t>
+  </si>
+  <si>
+    <t>L</t>
   </si>
 </sst>
 </file>
@@ -377,10 +380,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -392,10 +395,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -781,46 +784,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
     </row>
     <row r="3" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
     </row>
     <row r="4" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -876,7 +879,7 @@
       </c>
       <c r="J5" s="6"/>
     </row>
-    <row r="6" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -937,10 +940,10 @@
       <c r="D8" s="6">
         <v>6</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="6"/>
+      <c r="F8" s="6">
         <v>5</v>
       </c>
-      <c r="F8" s="6"/>
       <c r="G8" s="6">
         <v>7</v>
       </c>
@@ -989,9 +992,11 @@
       <c r="D10" s="6">
         <v>4</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6">
+      <c r="E10" s="6">
         <v>5</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="G10" s="6">
         <v>3</v>
@@ -1083,7 +1088,7 @@
         <v>6</v>
       </c>
       <c r="H13" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I13" s="6">
         <v>7</v>
@@ -1137,10 +1142,12 @@
       <c r="F15" s="6">
         <v>7</v>
       </c>
-      <c r="G15" s="6">
-        <v>2</v>
-      </c>
-      <c r="H15" s="6"/>
+      <c r="G15" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H15" s="6">
+        <v>1</v>
+      </c>
       <c r="I15" s="6">
         <v>4</v>
       </c>
@@ -1153,26 +1160,24 @@
       <c r="B16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>62</v>
+      <c r="C16" s="13">
+        <v>2</v>
       </c>
       <c r="D16" s="2">
+        <v>7</v>
+      </c>
+      <c r="E16" s="6">
+        <v>7</v>
+      </c>
+      <c r="F16" s="6">
         <v>2</v>
       </c>
-      <c r="E16" s="6">
-        <v>7</v>
-      </c>
-      <c r="F16" s="6">
-        <v>7</v>
-      </c>
       <c r="G16" s="6">
-        <v>2</v>
-      </c>
-      <c r="H16" s="6">
         <v>4</v>
       </c>
+      <c r="H16" s="6"/>
       <c r="I16" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J16" s="6"/>
     </row>
@@ -1183,7 +1188,7 @@
       <c r="B17" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="13" t="s">
         <v>62</v>
       </c>
       <c r="D17" s="7" t="s">
@@ -1213,7 +1218,7 @@
       <c r="B18" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>62</v>
       </c>
       <c r="D18" s="7" t="s">
@@ -1243,7 +1248,7 @@
       <c r="B19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="13" t="s">
         <v>62</v>
       </c>
       <c r="D19" s="7" t="s">
@@ -1273,7 +1278,7 @@
       <c r="B20" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="13" t="s">
         <v>62</v>
       </c>
       <c r="D20" s="7" t="s">
@@ -1303,7 +1308,7 @@
       <c r="B21" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="13" t="s">
         <v>62</v>
       </c>
       <c r="D21" s="7" t="s">
@@ -1333,7 +1338,7 @@
       <c r="B22" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="13" t="s">
         <v>62</v>
       </c>
       <c r="D22" s="6" t="s">
@@ -1363,20 +1368,18 @@
       <c r="B23" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="13" t="s">
         <v>62</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>7</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E23" s="6"/>
       <c r="F23" s="6">
-        <v>1</v>
-      </c>
-      <c r="G23" s="6">
         <v>4</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
@@ -1389,26 +1392,26 @@
       <c r="B24" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D24" s="6" t="s">
-        <v>62</v>
+      <c r="D24" s="6">
+        <v>1</v>
       </c>
       <c r="E24" s="6">
         <v>1</v>
       </c>
-      <c r="F24" s="6">
-        <v>4</v>
-      </c>
-      <c r="G24" s="6" t="s">
+      <c r="F24" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H24" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I24" s="6">
-        <v>1</v>
+      <c r="G24" s="6">
+        <v>2</v>
+      </c>
+      <c r="H24" s="6">
+        <v>3</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="J24" s="8"/>
     </row>
@@ -1419,7 +1422,7 @@
       <c r="B25" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="13" t="s">
         <v>62</v>
       </c>
       <c r="D25" s="7" t="s">
@@ -1449,7 +1452,7 @@
       <c r="B26" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="13" t="s">
         <v>62</v>
       </c>
       <c r="D26" s="7" t="s">
@@ -1468,7 +1471,7 @@
         <v>45</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="J26" s="8"/>
     </row>
@@ -1479,7 +1482,7 @@
       <c r="B27" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="13" t="s">
         <v>62</v>
       </c>
       <c r="D27" s="7" t="s">
@@ -1509,7 +1512,7 @@
       <c r="B28" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="13" t="s">
         <v>62</v>
       </c>
       <c r="D28" s="7" t="s">
@@ -1539,7 +1542,7 @@
       <c r="B29" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="13" t="s">
         <v>62</v>
       </c>
       <c r="D29" s="7" t="s">
@@ -1569,7 +1572,7 @@
       <c r="B30" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="13" t="s">
         <v>62</v>
       </c>
       <c r="D30" s="7" t="s">
@@ -1599,7 +1602,7 @@
       <c r="B31" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="13" t="s">
         <v>62</v>
       </c>
       <c r="D31" s="6" t="s">
@@ -1629,7 +1632,7 @@
       <c r="B32" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="13" t="s">
         <v>62</v>
       </c>
       <c r="D32" s="12" t="s">
@@ -1659,7 +1662,7 @@
       <c r="B33" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="13" t="s">
         <v>62</v>
       </c>
       <c r="D33" s="12" t="s">
@@ -1711,10 +1714,10 @@
       <c r="J35" s="19"/>
     </row>
     <row r="36" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="I36" s="18" t="s">
+      <c r="I36" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="J36" s="18"/>
+      <c r="J36" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>